<commit_message>
Updated ciphers to deal with validity dates and signature chains.
</commit_message>
<xml_diff>
--- a/Statistics/Calculate Samples and Errors.xlsx
+++ b/Statistics/Calculate Samples and Errors.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="140" windowWidth="18200" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16000" windowHeight="11480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,7 +342,7 @@
             <a:lstStyle/>
             <a:p>
               <a14:m>
-                <m:oMathPara xmlns="" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns="">
                   <m:oMathParaPr>
                     <m:jc m:val="centerGroup"/>
                   </m:oMathParaPr>
@@ -525,7 +525,7 @@
             <a:lstStyle/>
             <a:p>
               <a14:m>
-                <m:oMathPara xmlns="" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns="">
                   <m:oMathParaPr>
                     <m:jc m:val="centerGroup"/>
                   </m:oMathParaPr>
@@ -1561,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1581,7 +1581,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="4">
-        <v>4190</v>
+        <v>85000</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -1595,7 +1595,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="3">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="2:8">
@@ -1629,11 +1629,11 @@
       </c>
       <c r="G9" s="19">
         <f>D9*D9*(F5*(1-F5)/(F6* F6))</f>
-        <v>1691.265625</v>
+        <v>1268.44921875</v>
       </c>
       <c r="H9" s="20">
         <f>G9/(1+(G9/F3))</f>
-        <v>1204.9112249967454</v>
+        <v>1249.798559846098</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -1659,11 +1659,11 @@
       </c>
       <c r="G12" s="19">
         <f>D12*D12*(F5*(1-F5)/(F6* F6))</f>
-        <v>2401</v>
+        <v>1800.7499999999998</v>
       </c>
       <c r="H12" s="20">
         <f>G12/(1+(G12/F3))</f>
-        <v>1526.3526020330755</v>
+        <v>1763.3920213823035</v>
       </c>
     </row>
     <row r="13" spans="2:8">
@@ -1689,11 +1689,11 @@
       </c>
       <c r="G15" s="19">
         <f>D15*D15*(F5*(1-F5)/(F6* F6))</f>
-        <v>4144.1406250000009</v>
+        <v>3108.1054687500005</v>
       </c>
       <c r="H15" s="20">
         <f>G15/(1+(G15/F3))</f>
-        <v>2083.4720698932292</v>
+        <v>2998.4638012384912</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -1727,7 +1727,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="1">
-        <v>45</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1735,7 +1735,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="1">
-        <v>2</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="E22" s="2">
         <f>E21/E20</f>
-        <v>4.4444444444444446E-2</v>
+        <v>0.30952380952380953</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1771,7 +1771,7 @@
       <c r="D25" s="10"/>
       <c r="E25" s="2">
         <f>SQRT((E22)*(1-(E22))/E20)*D9</f>
-        <v>5.0535475594406076E-2</v>
+        <v>3.7107580801098486E-3</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="11"/>
@@ -1784,14 +1784,14 @@
       <c r="D26" s="13"/>
       <c r="E26" s="14">
         <f>E22-E25</f>
-        <v>-6.0910311499616301E-3</v>
+        <v>0.30581305144369969</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>7</v>
       </c>
       <c r="G26" s="15">
         <f>E22+E25</f>
-        <v>9.4979920038850529E-2</v>
+        <v>0.31323456760391938</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1815,7 +1815,7 @@
       <c r="D29" s="10"/>
       <c r="E29" s="2">
         <f>SQRT((E22)*(1-(E22))/E20)*D12</f>
-        <v>6.0212481559292347E-2</v>
+        <v>4.4213287763010959E-3</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="11"/>
@@ -1828,14 +1828,14 @@
       <c r="D30" s="13"/>
       <c r="E30" s="14">
         <f>E22-E29</f>
-        <v>-1.5768037114847901E-2</v>
+        <v>0.30510248074750845</v>
       </c>
       <c r="F30" s="23" t="s">
         <v>7</v>
       </c>
       <c r="G30" s="15">
         <f>E22+E29</f>
-        <v>0.1046569260037368</v>
+        <v>0.31394513830011062</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1859,7 +1859,7 @@
       <c r="D33" s="10"/>
       <c r="E33" s="2">
         <f>SQRT((E22)*(1-(E22))/E20)*D15</f>
-        <v>7.9105683681213165E-2</v>
+        <v>5.8086334688649613E-3</v>
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="11"/>
@@ -1872,14 +1872,14 @@
       <c r="D34" s="13"/>
       <c r="E34" s="14">
         <f>E22-E33</f>
-        <v>-3.4661239236768719E-2</v>
+        <v>0.30371517605494458</v>
       </c>
       <c r="F34" s="23" t="s">
         <v>7</v>
       </c>
       <c r="G34" s="15">
         <f>E22+E33</f>
-        <v>0.1235501281256576</v>
+        <v>0.31533244299267449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>